<commit_message>
Correct discription for release on Github
</commit_message>
<xml_diff>
--- a/8seneca_Task assignment_ANSWER.xlsx
+++ b/8seneca_Task assignment_ANSWER.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\8seneca\Release-20250511-AnPV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D828629-32F5-4DCE-B41E-DC1E2229E55E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B15A2F1-1DB5-4060-BE00-68C6AFE2CCBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>TT</t>
   </si>
@@ -58,6 +58,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Answer (</t>
     </r>
@@ -67,6 +68,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>AnPV's discription</t>
     </r>
@@ -76,6 +78,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -90,6 +93,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>1. Domain Model</t>
     </r>
@@ -98,6 +102,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
  User (e.g. id, username, fullName)
@@ -116,6 +121,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 Suppose it is a </t>
@@ -125,6 +131,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>small DB</t>
     </r>
@@ -133,6 +140,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> (for demo)
 So tables contain maximum number of records is 2,147,483,647 (ID field type is int4)
@@ -146,6 +154,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>users</t>
     </r>
@@ -154,6 +163,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: contain user information with field size restriction such as user_name, full_name
 - </t>
@@ -164,6 +174,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>tasks_detail</t>
     </r>
@@ -172,6 +183,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: contains specific working items with different categories such as (Bug or Feature)
    depend on working item type some fields contain data such as Bug (bug_severity, bug_steps_to_reproduce) 
@@ -184,6 +196,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>tasks</t>
     </r>
@@ -192,6 +205,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: working item after assigned to specific user so called task. contain information about progress such as (OPEN, IN_PROGRESS, DONE)..
 </t>
@@ -200,10 +214,53 @@
   <si>
     <r>
       <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Sheet "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DB Model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">"
+- Scripts to create database in source directory: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   src\main\resources\db\migration</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>2. REST Endpoints</t>
     </r>
@@ -212,6 +269,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 Create standard CRUD (Create, Read, Update, Delete) operations for both User
@@ -225,6 +283,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> User</t>
     </r>
@@ -233,6 +292,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 o Create a user
@@ -248,6 +308,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">APIs are designed to simple check valid input and perform requirement function (assume that one task can be assigned to many users, but one task can not be assigned to someone twice).
 Standardize that HTTP content type of input is form-data type, and output is JSON.
@@ -261,6 +322,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Results as following:</t>
     </r>
@@ -269,6 +331,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 o Create a user:
@@ -279,6 +342,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">   POST /users/new</t>
     </r>
@@ -287,6 +351,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 o Get a user by id
@@ -297,6 +362,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> GET users/:id</t>
     </r>
@@ -305,6 +371,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 o List all users
@@ -315,6 +382,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">   GET /users</t>
     </r>
@@ -323,6 +391,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 o Update a user (e.g., fullName)
@@ -333,6 +402,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">   PUT users/:id</t>
     </r>
@@ -341,6 +411,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 o Delete a user
@@ -351,6 +422,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">   DELETE users/:id</t>
     </r>
@@ -361,44 +433,51 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">- Source: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Source\hsm-service_FEATURE_Test.zip</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">
-- Postman file: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Docs\Postman.json</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Source on github</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: 
+    https://github.com/Golden-Man-Vn/hsm-service_FEATURE_Test.git</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- Postman file in source directory: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    Postman.json</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> Task</t>
     </r>
@@ -407,6 +486,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 o Create a task (assign to a user). Must handle the distinct fields based on the
@@ -423,6 +503,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">"Task" as required is divided into two items: Tasks_Detail and Tasks. 
 So APIs also seperated into 2 parts
@@ -434,6 +515,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Results for Tasks_Detail :
 </t>
@@ -443,6 +525,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">o Create a task (assign to a user). Must handle the distinct fields based on the
 category (e.g., severity, deadline, etc.).
@@ -454,6 +537,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">   -  </t>
     </r>
@@ -462,6 +546,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Create a detail:
 </t>
@@ -471,6 +556,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">   POST /tasks-detail/bug/new
    POST /tasks-detail/feature/new
@@ -481,6 +567,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">   - assign to a user:</t>
     </r>
@@ -490,15 +577,17 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">   POST /tasks/assign</t>
     </r>
@@ -507,6 +596,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 o Get a task by id
@@ -517,6 +607,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">   GET /tasks/:id</t>
     </r>
@@ -525,6 +616,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
   </t>
@@ -534,6 +626,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> GET /tasks-detail/:id</t>
     </r>
@@ -542,6 +635,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 o List all tasks
@@ -552,6 +646,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">   GET /tasks
    GET /tasks-detail
@@ -562,6 +657,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">o Update a task (including category-specific fields)
 </t>
@@ -571,6 +667,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">   PUT /tasks-detail/bug/:id
    PUT /tasks-detail/feature/:id
@@ -581,6 +678,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">  - change assign to a user or update progress:</t>
     </r>
@@ -589,6 +687,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
    PUT /tasks/:id</t>
@@ -598,6 +697,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 o Delete a task
@@ -608,6 +708,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">   DELETE /tasks-detail/:id
    DELETE /tasks/:id</t>
@@ -619,44 +720,51 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">- Source: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Source\hsm-service_FEATURE_Test.zip</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">
-- Postman file: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Docs\Postman.json</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Source on github</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: 
+    https://github.com/Golden-Man-Vn/hsm-service_FEATURE_Test.git</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- Postman file in source directory: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    Postman.json</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>3. Filtering &amp; Searching</t>
     </r>
@@ -665,6 +773,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
  Provide a way to filter tasks by:
@@ -679,6 +788,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Provide ability filter (search) like excel columns filter. It means that any field is input then search perform on this field and perform AND operator with the result of another field.
 </t>
@@ -689,6 +799,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Results as following:</t>
     </r>
@@ -697,15 +808,17 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>/users/search</t>
     </r>
@@ -716,44 +829,51 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">- Source: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Source\hsm-service_FEATURE_Test.zip</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">
-- Postman file: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Docs\Postman.json</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Source on github</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: 
+    https://github.com/Golden-Man-Vn/hsm-service_FEATURE_Test.git</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- Postman file in source directory: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    Postman.json</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">4. Migrations
 </t>
@@ -763,6 +883,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> Use Flyway or Liquibase to manage database schema changes.
  Create separate migration scripts for User and Task (including the two
@@ -775,6 +896,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
  Use Flyway or Liquibase to manage database schema changes.
@@ -785,6 +907,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">    Flyway integrated.
 </t>
@@ -794,6 +917,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">    </t>
     </r>
@@ -802,6 +926,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Limitation: 
          current project integrated DBs are Neon or Supabase Postgres DB (online DB)
@@ -814,6 +939,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>application.yml</t>
     </r>
@@ -822,6 +948,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> file by default
          I tested scripts manually by running on Neon Postgres DB well, 
@@ -832,6 +959,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
  Create separate migration scripts for User and Task (including the two
@@ -843,6 +971,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">    Scripts is written down</t>
     </r>
@@ -853,26 +982,30 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">- Scripts to create database in source code: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Source\hsm-service_FEATURE_Test\src\main\resources\db\migration</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- Scripts to create database in source directory: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>src\main\resources\db\migration</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">5. Error Handling
 </t>
@@ -882,6 +1015,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> Return proper HTTP status codes (e.g., 404 for not found, 400 for bad request).
  Provide meaningful error messages in JSON when requests fail.</t>
@@ -900,10 +1034,54 @@
   <si>
     <r>
       <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Source on github</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: 
+    https://github.com/Golden-Man-Vn/hsm-service_FEATURE_Test.git</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- Postman file in source directory: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    Postman.json</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">6. Testing
 </t>
@@ -913,6 +1091,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> Use JUnit (or another framework) to create at least some unit tests.
  If time permits, create at least one integration test that checks end-to-end
@@ -925,6 +1104,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Use JUnit (or another framework) to create at least some unit tests.
     </t>
@@ -934,6 +1114,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Some JUnit test cases for create tasks (task detail) and users
     Then perform assign task to someone  automatically if they are free (if user or task not free, try someone or task randomically)</t>
@@ -943,6 +1124,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> 
  If time permits, create at least one integration test that checks end-to-end
@@ -954,6 +1136,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">     Beacause of time limitation so it left remain (not to be done)</t>
     </r>
@@ -964,25 +1147,29 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">- Source: java class is placed at: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Source\hsm-service_FEATURE_Test\src\main\java\com\company\project\test</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- Source: java class is placed at directory: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>src\main\java\com\company\project\test</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">7. Documentation
 </t>
@@ -1002,6 +1189,7 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>README.md</t>
     </r>
@@ -1023,6 +1211,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Documents for reference:
 - README.md
@@ -1034,6 +1223,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>8seneca_Task assignment_ANSWER.xlsx</t>
     </r>
@@ -1043,6 +1233,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -1052,6 +1243,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">   https://docs.google.com/spreadsheets/d/1qghY4qz9eqOIuHN_iU7i4cyM5-w40dJANRmGZhH0XjU/edit?usp=sharing </t>
     </r>
@@ -1062,9 +1254,29 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Documents for reference:
-- README.md
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>README.md</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
 - This file (online or attachment for diliverables): </t>
     </r>
     <r>
@@ -1073,6 +1285,7 @@
         <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>8seneca_Task assignment_ANSWER.xlsx</t>
     </r>
@@ -1082,6 +1295,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -1091,6 +1305,7 @@
         <sz val="10"/>
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">   https://docs.google.com/spreadsheets/d/1qghY4qz9eqOIuHN_iU7i4cyM5-w40dJANRmGZhH0XjU/edit?usp=sharing </t>
     </r>
@@ -1139,67 +1354,13 @@
   </si>
   <si>
     <t>feature_deadline</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Refer to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>sheet "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>DB Model</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">"
-- scripts to create database in source code: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Source\hsm-service_FEATURE_Test\src\main\resources\db\migration</t>
-    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1211,12 +1372,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1224,78 +1387,84 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1427,7 +1596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1437,6 +1606,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1472,7 +1647,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1696,14 +1871,14 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="60.5703125" customWidth="1"/>
-    <col min="3" max="3" width="68.5703125" customWidth="1"/>
+    <col min="3" max="3" width="49" customWidth="1"/>
     <col min="4" max="4" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1721,8 +1896,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="229.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="22">
+    <row r="2" spans="1:4" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="24">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1731,205 +1906,206 @@
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="255" x14ac:dyDescent="0.2">
-      <c r="A3" s="22">
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="273" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="24">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="352.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="24">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="267.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="24">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="191.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="24">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="165.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="24">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="318.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="22">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="24">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="22">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="191.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="22">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="165.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="22">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="A8" s="22">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9" s="22">
-        <v>9</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>23</v>
+      <c r="B9" s="25" t="s">
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="22"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="22"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="22"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="22"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="22"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="22"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="22"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="22"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="22"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
+      <c r="A25" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1952,128 +2128,128 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="20" t="s">
+      <c r="B3" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="21"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="23"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="23"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9">
+      <c r="B4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11">
         <v>1</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="13">
+      <c r="E4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="15">
         <v>1</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="8"/>
+      <c r="J4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="10"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="8"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="10"/>
     </row>
     <row r="6" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="14" t="s">
+      <c r="B6" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="8"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="10"/>
     </row>
     <row r="7" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="19"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="K7" s="8"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="10"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="8"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="10"/>
     </row>
     <row r="9" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J9" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="8"/>
+      <c r="J9" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="10"/>
     </row>
     <row r="10" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J10" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="K10" s="8"/>
+      <c r="J10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>